<commit_message>
Bristol Data and laser lock changes
</commit_message>
<xml_diff>
--- a/DataAnalysis/2021-07-27trial20.xlsx
+++ b/DataAnalysis/2021-07-27trial20.xlsx
@@ -8,14 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charlottezehnder/Documents/laserStabilization/DataAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2A0ACF7-11AF-D94E-9534-D2E1087DB282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{BC2A5899-90E5-944B-A9A6-63CE5F11DE95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16740"/>
+    <workbookView xWindow="800" yWindow="460" windowWidth="17120" windowHeight="16740"/>
   </bookViews>
   <sheets>
     <sheet name="2021-07-27trial20" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -585,6 +596,1185 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2021-07-27trial20'!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> Frequency Drift (GHz)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'2021-07-27trial20'!$A$7:$A$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>2.117</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.456</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32.792999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>48.13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>63.488999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>78.832999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>94.176000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>109.51</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>124.864</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>140.20400000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>155.53800000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>170.87700000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>186.232</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>201.57400000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>216.91499999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>232.24299999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>247.59800000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>262.93700000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>278.27</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>293.59899999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>308.94200000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>324.28199999999998</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>339.62400000000002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>354.96</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>370.30399999999997</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>385.64400000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>400.97899999999998</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>416.31799999999998</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>431.66199999999998</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>447</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>462.339</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>477.673</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>493.04</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>508.37099999999998</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>523.70899999999995</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>539.04399999999998</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>554.39599999999996</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>569.73099999999999</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>585.06200000000001</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>600.40300000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'2021-07-27trial20'!$B$7:$B$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="40"/>
+                <c:pt idx="0">
+                  <c:v>-3.7380629707795799E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-8.8778995556015108E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-7.4761259415591702E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.07469310409913E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-4.6725787134744802E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-5.6070944561693696E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-9.3451574269489603E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-9.8124152982964098E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-8.8778995556015108E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-5.1398365848219297E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-5.1398365848219297E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-5.1398365848219297E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-7.4761259415591702E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-5.6070944561693696E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-6.07435232751682E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-6.5416101988642703E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.6725787134744802E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.3451574269489595E-4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.3362893567372401E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-7.9433838129066101E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.6725787134744802E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.3451574269489595E-4</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-9.3451574269489603E-3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.40177361404234E-3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.8690314853897899E-3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-3.7380629707795799E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-3.7380629707795799E-3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-8.8778995556015108E-3</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-5.6070944561693696E-3</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-9.3451574269489603E-3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-9.8124152982964098E-3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-7.0088680702117198E-3</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4.6725787134744797E-4</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-9.8124152982964098E-3</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-8.8778995556015108E-3</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-9.8124152982964098E-3</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-6.5416101988642703E-3</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-8.8778995556015108E-3</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-7.0088680702117198E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-931F-A646-B3EB-163C2BB139F3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1789120992"/>
+        <c:axId val="1724863952"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1789120992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1724863952"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1724863952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1789120992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>82550</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D99098F-8CF1-BA4D-B30D-CAE0AFA4A658}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -886,7 +2076,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E10" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:B46"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -1383,5 +2575,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>